<commit_message>
Se agregó las librerías para gestionar usuarios en el Domain. Se corrigó un error de visualización del monto total de un archivo importado. Se corrigió un error al guardar el monto de un concepto en el mantenimiento de datos externos.
</commit_message>
<xml_diff>
--- a/docs/Formato carga valores externos de conceptos.xlsx
+++ b/docs/Formato carga valores externos de conceptos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HUMBERTO-PC\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FB0304-6D3D-4407-9607-8766D901720A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BD5FB4-11EA-4D68-8B92-2795F6B9B98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8A22229E-7FFA-4F20-BBFA-6FC8C3493951}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>año</t>
   </si>
@@ -59,10 +59,19 @@
     <t>proveedor</t>
   </si>
   <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>categoria</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>72656577</t>
   </si>
   <si>
-    <t>019</t>
+    <t>72656578</t>
   </si>
 </sst>
 </file>
@@ -415,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B63788-36CB-42E9-8343-303570BCA300}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,12 +436,13 @@
     <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,16 +456,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -466,19 +479,22 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2">
+      <c r="G2">
         <v>75</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2023</v>
       </c>
@@ -489,338 +505,19 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3">
-        <v>124</v>
-      </c>
       <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2023</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4">
         <v>75</v>
       </c>
-      <c r="G4">
+      <c r="H3">
         <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2023</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5">
-        <v>123</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2023</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6">
-        <v>43</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2023</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7">
-        <v>124</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2023</v>
-      </c>
-      <c r="B8">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8">
-        <v>45</v>
-      </c>
-      <c r="G8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2023</v>
-      </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9">
-        <v>512</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2023</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10">
-        <v>213</v>
-      </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2023</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11">
-        <v>512</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2023</v>
-      </c>
-      <c r="B12">
-        <v>6</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12">
-        <v>213</v>
-      </c>
-      <c r="G12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2023</v>
-      </c>
-      <c r="B13">
-        <v>6</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13">
-        <v>124</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2023</v>
-      </c>
-      <c r="B14">
-        <v>7</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14">
-        <v>432</v>
-      </c>
-      <c r="G14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2023</v>
-      </c>
-      <c r="B15">
-        <v>7</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15">
-        <v>2412</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2023</v>
-      </c>
-      <c r="B16">
-        <v>8</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16">
-        <v>2</v>
-      </c>
-      <c r="G16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>2023</v>
-      </c>
-      <c r="B17">
-        <v>8</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>